<commit_message>
LUZ AMA A BRAULIO
</commit_message>
<xml_diff>
--- a/output/diccionario_andino_por_tabla.xlsx
+++ b/output/diccionario_andino_por_tabla.xlsx
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="n">
         <v>16384</v>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
         <v>16384</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>origen</t>
+          <t>origen_iata</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>destino</t>
+          <t>destino_iata</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -5852,7 +5852,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>origen</t>
+          <t>origen_iata</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>destino</t>
+          <t>destino_iata</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">

</xml_diff>